<commit_message>
Alteração de notas com sorteio das duplas para ultima avaliação.
</commit_message>
<xml_diff>
--- a/Linguagens II - planilha de notas.xlsx
+++ b/Linguagens II - planilha de notas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>Nota1</t>
   </si>
@@ -58,13 +58,31 @@
     <t>Nota2</t>
   </si>
   <si>
-    <t>Fechamento:</t>
-  </si>
-  <si>
     <t>7.5</t>
   </si>
   <si>
     <t>5.5</t>
+  </si>
+  <si>
+    <t>Nota3</t>
+  </si>
+  <si>
+    <t>Faltas</t>
+  </si>
+  <si>
+    <t>threds</t>
+  </si>
+  <si>
+    <t>Cliente Servidor (soap xml - web services)</t>
+  </si>
+  <si>
+    <t>Cliente Servidor (restfull json - web services)</t>
+  </si>
+  <si>
+    <t>Inser no banco usando arquitetura MVC</t>
+  </si>
+  <si>
+    <t>Inser no banco usando arquitetura em 3 camadas</t>
   </si>
 </sst>
 </file>
@@ -88,7 +106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +119,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -193,40 +235,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -322,15 +334,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -340,35 +374,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,183 +720,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16">
+        <v>4</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16">
+        <v>4</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="H5" s="24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16">
+        <v>4</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <v>8</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>16</v>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16">
+        <v>4</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16">
+        <v>4</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E10" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17">
+        <v>4</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Inclussão da nota de wellington
</commit_message>
<xml_diff>
--- a/Linguagens II - planilha de notas.xlsx
+++ b/Linguagens II - planilha de notas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Nota1</t>
   </si>
@@ -387,15 +387,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -414,6 +405,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -723,7 +723,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,21 +734,21 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="16" t="s">
         <v>10</v>
       </c>
     </row>
@@ -763,12 +763,12 @@
       <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="24" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -786,11 +786,11 @@
       <c r="E3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13">
         <v>4</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
     </row>
@@ -808,11 +808,11 @@
       <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13">
         <v>4</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="18" t="s">
         <v>20</v>
       </c>
     </row>
@@ -830,11 +830,11 @@
       <c r="E5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13">
         <v>4</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -852,11 +852,11 @@
       <c r="E6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16">
+      <c r="F6" s="13"/>
+      <c r="G6" s="13">
         <v>4</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -874,11 +874,11 @@
       <c r="E7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13">
         <v>8</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -896,11 +896,11 @@
       <c r="E8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13">
         <v>4</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -915,12 +915,14 @@
       <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16">
+      <c r="E9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13">
         <v>4</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -938,11 +940,11 @@
       <c r="E10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14">
         <v>4</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="20" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
incluindo a segunda nota da primeira avaliação.
</commit_message>
<xml_diff>
--- a/Linguagens II - planilha de notas.xlsx
+++ b/Linguagens II - planilha de notas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
   <si>
     <t>Nota1</t>
   </si>
@@ -723,7 +723,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,9 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
@@ -779,7 +781,9 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
@@ -801,7 +805,9 @@
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
@@ -823,7 +829,9 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
@@ -845,7 +853,9 @@
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
@@ -867,7 +877,9 @@
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
@@ -889,7 +901,9 @@
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
@@ -911,7 +925,9 @@
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
@@ -933,7 +949,9 @@
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Incluido campo de peso para as notas das avaliações
</commit_message>
<xml_diff>
--- a/Linguagens II - planilha de notas.xlsx
+++ b/Linguagens II - planilha de notas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
   <si>
     <t>Nota1</t>
   </si>
@@ -83,13 +83,16 @@
   </si>
   <si>
     <t>Inser no banco usando arquitetura em 3 camadas</t>
+  </si>
+  <si>
+    <t>Peso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,8 +108,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +154,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -374,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -416,6 +433,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,6 +989,26 @@
         <v>22</v>
       </c>
     </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="26">
+        <v>2</v>
+      </c>
+      <c r="C11" s="27">
+        <v>2</v>
+      </c>
+      <c r="D11" s="26">
+        <v>2</v>
+      </c>
+      <c r="E11" s="27">
+        <v>2</v>
+      </c>
+      <c r="F11" s="28">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>

</xml_diff>